<commit_message>
Crea Excel con 2 hojas sin index
</commit_message>
<xml_diff>
--- a/pandas/output/reporte.xlsx
+++ b/pandas/output/reporte.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Colores" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Ciudades" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,145 +435,316 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ID_COLOR</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>ID_COLOR</t>
+          <t>Color</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Blanco</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Negro</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Rojo</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Verde</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Azul</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Amarillo</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Celeste</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Rosado</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Marron</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Naranja</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ID_EDIFICIO</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Nombre</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Color</t>
+          <t>Ranking</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>El Pinar</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Alameda</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Carolina</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Cumanda</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Chambo</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
         <v>1</v>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Blanco</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Ambato</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
         <v>2</v>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Negro</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>3</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Rojo</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="n">
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Riobamba</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>h</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Guayaquil</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
         <v>4</v>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Verde</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="n">
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>i</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Quito</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
         <v>5</v>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Azul</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="n">
-        <v>6</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Amarillo</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="n">
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>j</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Cuenca</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
         <v>7</v>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Celeste</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="n">
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>k</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Machala</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
         <v>8</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Rosado</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="n">
-        <v>9</v>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Marron</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="n">
-        <v>10</v>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Naranja</t>
-        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>